<commit_message>
loaded player data as dict, began util functions
</commit_message>
<xml_diff>
--- a/test_players.xlsx
+++ b/test_players.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jingqi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jingqi/Desktop/teampartition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48F7F0B-2201-3B40-8DD5-92FC1570E674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F930EA-BE49-0249-A5C1-CC074AEAAF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="27980" windowHeight="18380" xr2:uid="{8F58AEF8-0A0C-344B-AB88-3ED362C15D30}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2025" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>

<commit_message>
convert yankee rating to numerical score
</commit_message>
<xml_diff>
--- a/test_players.xlsx
+++ b/test_players.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jingqi/Desktop/teampartition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F930EA-BE49-0249-A5C1-CC074AEAAF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF3B105-775A-F547-AB32-8AC57B90B457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="27980" windowHeight="18380" xr2:uid="{8F58AEF8-0A0C-344B-AB88-3ED362C15D30}"/>
   </bookViews>
@@ -690,7 +690,7 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>

</xml_diff>